<commit_message>
WIP updating inputs and interface
</commit_message>
<xml_diff>
--- a/Province snapshot info.xlsx
+++ b/Province snapshot info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/31049984142acc5a/Dev/utopia-province-sim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{14D64161-EECC-41B0-8CE8-2F1251D8221E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{14D64161-EECC-41B0-8CE8-2F1251D8221E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2FF6226-8D9F-47D4-8776-6FA06B708585}"/>
   <bookViews>
-    <workbookView xWindow="370" yWindow="240" windowWidth="12100" windowHeight="14810" xr2:uid="{C8E1AD5E-9B77-4715-AB82-E49B56C7E4D8}"/>
+    <workbookView xWindow="12510" yWindow="230" windowWidth="12110" windowHeight="14810" xr2:uid="{C8E1AD5E-9B77-4715-AB82-E49B56C7E4D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="297">
   <si>
     <t>Data</t>
   </si>
@@ -122,9 +122,6 @@
     <t>Army</t>
   </si>
   <si>
-    <t>Wizard</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -209,16 +206,7 @@
     <t>Total Population</t>
   </si>
   <si>
-    <t xml:space="preserve">Peasant Population </t>
-  </si>
-  <si>
-    <t>Wizard Population</t>
-  </si>
-  <si>
     <t>Military &amp; Thief Population</t>
-  </si>
-  <si>
-    <t>Number of Soldiers</t>
   </si>
   <si>
     <t>Free Specialist Credits Left</t>
@@ -1331,8 +1319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67B7DCB5-B338-4263-A5AD-AE714D64F106}">
   <dimension ref="B1:C230"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1346,7 +1334,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="2:3" ht="18.5" x14ac:dyDescent="0.45">
@@ -1359,7 +1347,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.35">
@@ -1367,7 +1355,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.35">
@@ -1375,7 +1363,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.35">
@@ -1383,7 +1371,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.35">
@@ -1391,7 +1379,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.35">
@@ -1399,15 +1387,15 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C9" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.35">
@@ -1415,7 +1403,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.35">
@@ -1423,7 +1411,7 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.35">
@@ -1431,7 +1419,7 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.35">
@@ -1439,7 +1427,7 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.35">
@@ -1447,7 +1435,7 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.35">
@@ -1455,7 +1443,7 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.35">
@@ -1463,7 +1451,7 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.35">
@@ -1471,7 +1459,7 @@
         <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.35">
@@ -1479,7 +1467,7 @@
         <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.35">
@@ -1487,7 +1475,7 @@
         <v>17</v>
       </c>
       <c r="C20" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.35">
@@ -1495,7 +1483,7 @@
         <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.35">
@@ -1503,7 +1491,7 @@
         <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.35">
@@ -1511,7 +1499,7 @@
         <v>20</v>
       </c>
       <c r="C23" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.35">
@@ -1519,7 +1507,7 @@
         <v>21</v>
       </c>
       <c r="C24" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.35">
@@ -1527,7 +1515,7 @@
         <v>22</v>
       </c>
       <c r="C25" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.35">
@@ -1535,7 +1523,7 @@
         <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.35">
@@ -1543,15 +1531,15 @@
         <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C29" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="31" spans="2:3" ht="18.5" x14ac:dyDescent="0.45">
@@ -1569,7 +1557,7 @@
         <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.35">
@@ -1577,7 +1565,7 @@
         <v>27</v>
       </c>
       <c r="C34" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.35">
@@ -1585,36 +1573,36 @@
         <v>19</v>
       </c>
       <c r="C35" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C36" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C37" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C38" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B40" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.35">
@@ -1622,446 +1610,446 @@
         <v>8</v>
       </c>
       <c r="C41" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C42" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C43" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C44" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C45" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C46" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B48" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C49" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C50" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C51" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C52" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B54" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C54" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B55" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C55" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B56" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C56" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B57" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C57" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B58" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C58" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B60" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C60" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B61" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C61" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B62" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C62" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="64" spans="2:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B64" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B65" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C65" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B66" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C66" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B67" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C67" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B68" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C68" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B69" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C69" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B71" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C71" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B72" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="C72" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B73" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="C73" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B74" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C74" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B75" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="C75" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B76" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C76" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B77" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C77" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B78" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C78" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B79" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C79" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B81" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C81" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B82" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C82" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B83" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C83" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B84" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C84" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B85" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C85" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B86" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C86" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B87" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C87" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B88" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C88" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B89" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C89" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B90" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C90" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B91" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C91" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B92" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C92" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B93" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C93" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B94" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C94" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B95" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C95" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B96" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C96" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B97" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C97" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B98" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C98" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B99" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C99" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B100" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C100" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="103" spans="2:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B103" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B104" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C104" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B105" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C105" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.35">
@@ -2069,972 +2057,972 @@
         <v>9</v>
       </c>
       <c r="C106" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B107" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C107" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="108" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B108" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C108" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B109" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C109" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B110" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C110" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B111" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C111" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B112" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C112" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="113" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B113" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C113" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B114" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C114" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B115" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C115" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B117" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C117" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="118" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B118" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C118" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="119" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B119" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C119" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="120" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B120" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C120" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="121" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B121" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C121" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="122" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B122" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C122" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="123" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B123" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C123" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="124" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B124" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C124" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="125" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B125" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C125" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="126" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B126" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C126" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="127" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B127" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C127" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="128" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B128" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C128" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="129" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B129" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C129" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="130" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B130" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C130" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="131" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B131" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C131" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="132" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B132" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C132" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="133" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B133" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C133" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="134" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B134" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C134" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="135" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B135" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C135" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="136" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B136" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C136" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="137" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B137" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C137" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="138" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B138" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C138" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="139" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B139" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C139" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="140" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B140" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C140" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="141" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B141" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C141" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="142" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B142" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C142" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="143" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B143" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C143" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="144" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B144" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C144" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="145" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B145" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C145" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="146" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B146" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C146" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="147" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B147" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C147" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="148" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B148" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C148" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="149" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B149" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C149" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="150" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B150" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C150" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="151" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B151" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C151" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="152" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B152" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C152" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="153" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B153" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C153" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="154" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B154" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C154" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="155" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B155" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C155" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="156" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B156" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C156" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="157" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B157" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C157" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="158" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B158" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C158" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="159" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B159" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C159" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="160" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B160" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C160" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="161" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B161" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C161" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="162" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B162" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C162" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="163" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B163" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C163" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="164" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B164" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C164" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="165" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B165" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C165" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="166" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B166" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C166" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="167" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B167" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C167" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="168" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B168" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C168" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="169" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B169" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C169" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="170" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B170" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C170" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="171" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B171" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C171" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="172" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B172" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C172" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="173" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B173" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C173" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="174" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B174" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C174" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="175" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B175" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C175" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="176" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B176" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C176" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="177" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B177" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C177" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="178" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B178" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C178" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="179" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B179" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C179" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="180" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B180" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C180" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="181" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B181" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C181" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="182" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B182" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C182" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="183" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B183" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C183" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="184" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B184" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C184" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="185" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B185" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C185" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="186" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B186" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C186" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="187" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B187" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C187" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="188" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B188" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C188" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="189" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B189" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C189" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="190" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B190" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C190" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="191" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B191" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C191" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="194" spans="2:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B194" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="195" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B195" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C195" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="196" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B196" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C196" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="197" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B197" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C197" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="198" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B198" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C198" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="199" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B199" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C199" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="200" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B200" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C200" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="201" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B201" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C201" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="202" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B202" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C202" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="203" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B203" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C203" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="204" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B204" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C204" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="205" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B205" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C205" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="206" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B206" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C206" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="207" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B207" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C207" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="208" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B208" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C208" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="209" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B209" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C209" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="210" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B210" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C210" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="211" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B211" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C211" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="212" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B212" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C212" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="213" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B213" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C213" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="214" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B214" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C214" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="215" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B215" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C215" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="216" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B216" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C216" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="217" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B217" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C217" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="218" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B218" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C218" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="219" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B219" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C219" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="220" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B220" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C220" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="221" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B221" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C221" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="222" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B222" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C222" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="223" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B223" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C223" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="224" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B224" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C224" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="225" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B225" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C225" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="226" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B226" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C226" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="227" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B227" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C227" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="228" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B228" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C228" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="229" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B229" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C229" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="230" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B230" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C230" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>